<commit_message>
code clean and refactor
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/JumiaTestData.xlsx
+++ b/src/test/java/testdata/JumiaTestData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Tharwat\IdeaProjects\AutomationTask\src\test\java\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Tharwat\IdeaProjects\AutomationTaskAmazon\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1128600-76E6-4FC1-AECB-E71AC21ECC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F2883B-DDDD-4A47-9817-C72AE286AE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6EE9A35B-13FE-49F2-8E89-86D6A0ADD8B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Credentials" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Test@1234@</t>
   </si>
@@ -50,17 +50,35 @@
     <t>12201997</t>
   </si>
   <si>
-    <t>01122233325</t>
-  </si>
-  <si>
-    <t>jamefij283a0025@wiroute.com</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Birth Date in mm/dd/yy</t>
+  </si>
+  <si>
+    <t>jamefij283a0036@wiroute.com</t>
+  </si>
+  <si>
+    <t>01122233336</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +94,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -108,6 +140,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -424,47 +459,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C1F4CE-E13D-4827-8766-6B8A74B3C594}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{1178E333-9605-43F3-8FEF-F6C322AD0437}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{350E3FCD-EDA1-48F0-A79A-9DE4220068FD}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1178E333-9605-43F3-8FEF-F6C322AD0437}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{350E3FCD-EDA1-48F0-A79A-9DE4220068FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>